<commit_message>
refactor: Update MIGO Inclusão da leitura de dados da planilha Excel.
</commit_message>
<xml_diff>
--- a/Dados apresentação 22-08.xlsx
+++ b/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{696AA5FD-7EA9-402A-913C-FE6B79C161E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{696AA5FD-7EA9-402A-913C-FE6B79C161E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DCBE7F6-6C3F-491B-8DA0-AF9E499C0801}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView minimized="1" xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
-    <t>Pedido Origen</t>
-  </si>
-  <si>
     <t>Novo Pedido</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Z10</t>
+  </si>
+  <si>
+    <t>Pedido Origem</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,52 +535,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -588,16 +588,16 @@
         <v>4503273185</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>10001859</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
       <c r="G2">
         <v>5821</v>
@@ -609,13 +609,13 @@
         <v>2000</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <v>602.13800000000003</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2">
         <v>4600218517</v>
@@ -624,10 +624,10 @@
         <v>50</v>
       </c>
       <c r="O2" s="3">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -635,16 +635,16 @@
         <v>4503274856</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>10068989</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
       </c>
       <c r="G3">
         <v>5821</v>
@@ -656,13 +656,13 @@
         <v>2000</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3">
         <v>120</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3">
         <v>4600218433</v>
@@ -671,10 +671,10 @@
         <v>60</v>
       </c>
       <c r="O3" s="3">
-        <v>45899</v>
+        <v>45900</v>
       </c>
       <c r="P3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>